<commit_message>
Correction fichier excel pour valider min UCI, closes #11
- Validation du taux de change officiel UCI
- Validation des montants des étapes et demi-étape
- Validation de la règle du 20%
- Formattage conditionnel des cellules pour aider à trouver le minimum
</commit_message>
<xml_diff>
--- a/excel/prix.xlsx
+++ b/excel/prix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5A7E87-2005-394B-9448-61C722BA2D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCD025C-0CF2-3348-A65C-EB9EE195998C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="560" windowWidth="16720" windowHeight="20380" firstSheet="2" activeTab="8" xr2:uid="{CE5E1F58-89A2-BD42-AA5E-6DDAA3F3C6F4}"/>
+    <workbookView xWindow="60" yWindow="560" windowWidth="33480" windowHeight="20380" activeTab="9" xr2:uid="{CE5E1F58-89A2-BD42-AA5E-6DDAA3F3C6F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Etape" sheetId="3" r:id="rId1"/>
@@ -22,8 +22,9 @@
     <sheet name="GenEquipe" sheetId="7" r:id="rId7"/>
     <sheet name="Abitibien" sheetId="4" r:id="rId8"/>
     <sheet name="Total" sheetId="8" r:id="rId9"/>
+    <sheet name="Verif_UCI" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t>montant</t>
   </si>
@@ -89,13 +90,76 @@
   </si>
   <si>
     <t>GenJeune</t>
+  </si>
+  <si>
+    <t>Places</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Half</t>
+  </si>
+  <si>
+    <t>GC min</t>
+  </si>
+  <si>
+    <t>Min_UCI</t>
+  </si>
+  <si>
+    <t>Taux de change officiel UCI (https://assets.ctfassets.net/761l7gh5x5an/5G5JfslUY9ynE73LV2g9Zi/83a927bf79ee339a0df921fef64fe385/FX_officiel_UCI_2023_-_Multi.pdf)</t>
+  </si>
+  <si>
+    <t>Obligations minimales pour 2023</t>
+  </si>
+  <si>
+    <t>https://assets.ctfassets.net/761l7gh5x5an/4LhHQ0knlVpQFA1wf3X2Re/d6066b0cb0f95507c1117cf0e1afdb13/ROA-20220420_-_2023_Road_Financial_Obligations_-v2_PW_Lbo_Corrected_17.06.2022.pdf</t>
+  </si>
+  <si>
+    <t>Validation se fait en rouge si montant pas assez élevé, dans Onglets Etape, Demi-Étape, GenTemps</t>
+  </si>
+  <si>
+    <t>euro_min_UCI</t>
+  </si>
+  <si>
+    <t>CAD_conv_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --&gt; à mettre à jour annuellement en utilisant le taux de change UCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --&gt; à valider en fonction des montants officiels UCI dans "2023 - ROUTE Obligations Financières"</t>
+  </si>
+  <si>
+    <t>Étapes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,6 +171,36 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,17 +223,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -449,66 +596,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6883AF19-C74A-2446-B83A-283A67BC0B24}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>255</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>175</v>
+      </c>
+      <c r="D2" s="3">
+        <f>ROUNDUP(C2*Verif_UCI!$B$29,0)</f>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3" s="3">
+        <f>ROUNDUP(C3*Verif_UCI!$B$29,0)</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>75</v>
+      </c>
+      <c r="D4" s="3">
+        <f>ROUNDUP(C4*Verif_UCI!$B$29,0)</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5" s="3">
+        <f>ROUNDUP(C5*Verif_UCI!$B$29,0)</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3">
+        <f>ROUNDUP(C6*Verif_UCI!$B$29,0)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -516,17 +706,33 @@
         <f>B6</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f>C6</f>
+        <v>50</v>
+      </c>
+      <c r="D7" s="3">
+        <f>ROUNDUP(C7*Verif_UCI!$B$29,0)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B11" si="0">B7</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <f t="shared" ref="B8:C11" si="0">B7</f>
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D8" s="3">
+        <f>ROUNDUP(C8*Verif_UCI!$B$29,0)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -534,8 +740,16 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D9" s="3">
+        <f>ROUNDUP(C9*Verif_UCI!$B$29,0)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -543,8 +757,16 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D10" s="3">
+        <f>ROUNDUP(C10*Verif_UCI!$B$29,0)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -552,16 +774,31 @@
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D11" s="3">
+        <f>ROUNDUP(C11*Verif_UCI!$B$29,0)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3">
+        <f>ROUNDUP(C12*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -569,17 +806,33 @@
         <f>B12</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f>C12</f>
+        <v>20</v>
+      </c>
+      <c r="D13" s="3">
+        <f>ROUNDUP(C13*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:B21" si="1">B13</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <f t="shared" ref="B14:C21" si="1">B13</f>
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D14" s="3">
+        <f>ROUNDUP(C14*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -587,8 +840,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D15" s="3">
+        <f>ROUNDUP(C15*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -596,8 +857,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D16" s="3">
+        <f>ROUNDUP(C16*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -605,8 +874,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D17" s="3">
+        <f>ROUNDUP(C17*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -614,8 +891,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D18" s="3">
+        <f>ROUNDUP(C18*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -623,8 +908,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D19" s="3">
+        <f>ROUNDUP(C19*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -632,8 +925,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D20" s="3">
+        <f>ROUNDUP(C20*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -641,8 +942,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D21" s="3">
+        <f>ROUNDUP(C21*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -652,73 +961,1060 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B21">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>B2-D2 &lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7242B4-1C8C-8141-80D3-BFAEF59EC119}">
+  <dimension ref="A1:J34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>IF(B$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
+        <v>255</v>
+      </c>
+      <c r="C3">
+        <f>IF(C$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
+        <v>255</v>
+      </c>
+      <c r="D3">
+        <f>IF(D$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
+        <v>145</v>
+      </c>
+      <c r="E3">
+        <f>IF(E$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
+        <v>145</v>
+      </c>
+      <c r="F3">
+        <f>IF(F$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
+        <v>255</v>
+      </c>
+      <c r="G3">
+        <f>IF(G$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
+        <v>255</v>
+      </c>
+      <c r="H3">
+        <f>IF(H$2 = "FULL", Etape!$B2,DemiEtape!$B2)</f>
+        <v>255</v>
+      </c>
+      <c r="I3">
+        <f>SUM(B3:H3)</f>
+        <v>1565</v>
+      </c>
+      <c r="J3">
+        <f>I3*$J$2</f>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f>IF(B$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
+        <v>145</v>
+      </c>
+      <c r="C4">
+        <f>IF(C$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
+        <v>145</v>
+      </c>
+      <c r="D4">
+        <f>IF(D$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
+        <v>110</v>
+      </c>
+      <c r="E4">
+        <f>IF(E$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
+        <v>110</v>
+      </c>
+      <c r="F4">
+        <f>IF(F$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
+        <v>145</v>
+      </c>
+      <c r="G4">
+        <f>IF(G$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
+        <v>145</v>
+      </c>
+      <c r="H4">
+        <f>IF(H$2 = "FULL", Etape!$B3,DemiEtape!$B3)</f>
+        <v>145</v>
+      </c>
+      <c r="I4">
+        <f>SUM(B4:H4)</f>
+        <v>945</v>
+      </c>
+      <c r="J4">
+        <f>I4*$J$2</f>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f>IF(B$2 = "FULL", Etape!$B4,DemiEtape!$B4)</f>
+        <v>110</v>
+      </c>
+      <c r="C5">
+        <f>IF(C$2 = "FULL", Etape!$B4,DemiEtape!$B4)</f>
+        <v>110</v>
+      </c>
+      <c r="D5">
+        <f>IF(D$2 = "FULL", Etape!$B4,DemiEtape!$B4)</f>
+        <v>75</v>
+      </c>
+      <c r="E5">
+        <f>IF(E$2 = "FULL", Etape!$B4,DemiEtape!$B4)</f>
+        <v>75</v>
+      </c>
+      <c r="F5">
+        <f>IF(F$2 = "FULL", Etape!$B4,DemiEtape!$B4)</f>
+        <v>110</v>
+      </c>
+      <c r="G5">
+        <f>IF(G$2 = "FULL", Etape!$B4,DemiEtape!$B4)</f>
+        <v>110</v>
+      </c>
+      <c r="H5">
+        <f>IF(H$2 = "FULL", Etape!$B4,DemiEtape!$B4)</f>
+        <v>110</v>
+      </c>
+      <c r="I5">
+        <f>SUM(B5:H5)</f>
+        <v>700</v>
+      </c>
+      <c r="J5">
+        <f>I5*$J$2</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f>IF(B$2 = "FULL", Etape!$B5,DemiEtape!$B5)</f>
+        <v>90</v>
+      </c>
+      <c r="C6">
+        <f>IF(C$2 = "FULL", Etape!$B5,DemiEtape!$B5)</f>
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <f>IF(D$2 = "FULL", Etape!$B5,DemiEtape!$B5)</f>
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <f>IF(E$2 = "FULL", Etape!$B5,DemiEtape!$B5)</f>
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <f>IF(F$2 = "FULL", Etape!$B5,DemiEtape!$B5)</f>
+        <v>90</v>
+      </c>
+      <c r="G6">
+        <f>IF(G$2 = "FULL", Etape!$B5,DemiEtape!$B5)</f>
+        <v>90</v>
+      </c>
+      <c r="H6">
+        <f>IF(H$2 = "FULL", Etape!$B5,DemiEtape!$B5)</f>
+        <v>90</v>
+      </c>
+      <c r="I6">
+        <f>SUM(B6:H6)</f>
+        <v>570</v>
+      </c>
+      <c r="J6">
+        <f>I6*$J$2</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f>IF(B$2 = "FULL", Etape!$B6,DemiEtape!$B6)</f>
+        <v>75</v>
+      </c>
+      <c r="C7">
+        <f>IF(C$2 = "FULL", Etape!$B6,DemiEtape!$B6)</f>
+        <v>75</v>
+      </c>
+      <c r="D7">
+        <f>IF(D$2 = "FULL", Etape!$B6,DemiEtape!$B6)</f>
+        <v>45</v>
+      </c>
+      <c r="E7">
+        <f>IF(E$2 = "FULL", Etape!$B6,DemiEtape!$B6)</f>
+        <v>45</v>
+      </c>
+      <c r="F7">
+        <f>IF(F$2 = "FULL", Etape!$B6,DemiEtape!$B6)</f>
+        <v>75</v>
+      </c>
+      <c r="G7">
+        <f>IF(G$2 = "FULL", Etape!$B6,DemiEtape!$B6)</f>
+        <v>75</v>
+      </c>
+      <c r="H7">
+        <f>IF(H$2 = "FULL", Etape!$B6,DemiEtape!$B6)</f>
+        <v>75</v>
+      </c>
+      <c r="I7">
+        <f>SUM(B7:H7)</f>
+        <v>465</v>
+      </c>
+      <c r="J7">
+        <f>I7*$J$2</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f>IF(B$2 = "FULL", Etape!$B7,DemiEtape!$B7)</f>
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <f>IF(C$2 = "FULL", Etape!$B7,DemiEtape!$B7)</f>
+        <v>75</v>
+      </c>
+      <c r="D8">
+        <f>IF(D$2 = "FULL", Etape!$B7,DemiEtape!$B7)</f>
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <f>IF(E$2 = "FULL", Etape!$B7,DemiEtape!$B7)</f>
+        <v>45</v>
+      </c>
+      <c r="F8">
+        <f>IF(F$2 = "FULL", Etape!$B7,DemiEtape!$B7)</f>
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <f>IF(G$2 = "FULL", Etape!$B7,DemiEtape!$B7)</f>
+        <v>75</v>
+      </c>
+      <c r="H8">
+        <f>IF(H$2 = "FULL", Etape!$B7,DemiEtape!$B7)</f>
+        <v>75</v>
+      </c>
+      <c r="I8">
+        <f>SUM(B8:H8)</f>
+        <v>465</v>
+      </c>
+      <c r="J8">
+        <f>I8*$J$2</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f>IF(B$2 = "FULL", Etape!$B8,DemiEtape!$B8)</f>
+        <v>75</v>
+      </c>
+      <c r="C9">
+        <f>IF(C$2 = "FULL", Etape!$B8,DemiEtape!$B8)</f>
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <f>IF(D$2 = "FULL", Etape!$B8,DemiEtape!$B8)</f>
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <f>IF(E$2 = "FULL", Etape!$B8,DemiEtape!$B8)</f>
+        <v>45</v>
+      </c>
+      <c r="F9">
+        <f>IF(F$2 = "FULL", Etape!$B8,DemiEtape!$B8)</f>
+        <v>75</v>
+      </c>
+      <c r="G9">
+        <f>IF(G$2 = "FULL", Etape!$B8,DemiEtape!$B8)</f>
+        <v>75</v>
+      </c>
+      <c r="H9">
+        <f>IF(H$2 = "FULL", Etape!$B8,DemiEtape!$B8)</f>
+        <v>75</v>
+      </c>
+      <c r="I9">
+        <f>SUM(B9:H9)</f>
+        <v>465</v>
+      </c>
+      <c r="J9">
+        <f>I9*$J$2</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f>IF(B$2 = "FULL", Etape!$B9,DemiEtape!$B9)</f>
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <f>IF(C$2 = "FULL", Etape!$B9,DemiEtape!$B9)</f>
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <f>IF(D$2 = "FULL", Etape!$B9,DemiEtape!$B9)</f>
+        <v>45</v>
+      </c>
+      <c r="E10">
+        <f>IF(E$2 = "FULL", Etape!$B9,DemiEtape!$B9)</f>
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <f>IF(F$2 = "FULL", Etape!$B9,DemiEtape!$B9)</f>
+        <v>75</v>
+      </c>
+      <c r="G10">
+        <f>IF(G$2 = "FULL", Etape!$B9,DemiEtape!$B9)</f>
+        <v>75</v>
+      </c>
+      <c r="H10">
+        <f>IF(H$2 = "FULL", Etape!$B9,DemiEtape!$B9)</f>
+        <v>75</v>
+      </c>
+      <c r="I10">
+        <f>SUM(B10:H10)</f>
+        <v>465</v>
+      </c>
+      <c r="J10">
+        <f>I10*$J$2</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f>IF(B$2 = "FULL", Etape!$B10,DemiEtape!$B10)</f>
+        <v>75</v>
+      </c>
+      <c r="C11">
+        <f>IF(C$2 = "FULL", Etape!$B10,DemiEtape!$B10)</f>
+        <v>75</v>
+      </c>
+      <c r="D11">
+        <f>IF(D$2 = "FULL", Etape!$B10,DemiEtape!$B10)</f>
+        <v>45</v>
+      </c>
+      <c r="E11">
+        <f>IF(E$2 = "FULL", Etape!$B10,DemiEtape!$B10)</f>
+        <v>45</v>
+      </c>
+      <c r="F11">
+        <f>IF(F$2 = "FULL", Etape!$B10,DemiEtape!$B10)</f>
+        <v>75</v>
+      </c>
+      <c r="G11">
+        <f>IF(G$2 = "FULL", Etape!$B10,DemiEtape!$B10)</f>
+        <v>75</v>
+      </c>
+      <c r="H11">
+        <f>IF(H$2 = "FULL", Etape!$B10,DemiEtape!$B10)</f>
+        <v>75</v>
+      </c>
+      <c r="I11">
+        <f>SUM(B11:H11)</f>
+        <v>465</v>
+      </c>
+      <c r="J11">
+        <f>I11*$J$2</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f>IF(B$2 = "FULL", Etape!$B11,DemiEtape!$B11)</f>
+        <v>75</v>
+      </c>
+      <c r="C12">
+        <f>IF(C$2 = "FULL", Etape!$B11,DemiEtape!$B11)</f>
+        <v>75</v>
+      </c>
+      <c r="D12">
+        <f>IF(D$2 = "FULL", Etape!$B11,DemiEtape!$B11)</f>
+        <v>45</v>
+      </c>
+      <c r="E12">
+        <f>IF(E$2 = "FULL", Etape!$B11,DemiEtape!$B11)</f>
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <f>IF(F$2 = "FULL", Etape!$B11,DemiEtape!$B11)</f>
+        <v>75</v>
+      </c>
+      <c r="G12">
+        <f>IF(G$2 = "FULL", Etape!$B11,DemiEtape!$B11)</f>
+        <v>75</v>
+      </c>
+      <c r="H12">
+        <f>IF(H$2 = "FULL", Etape!$B11,DemiEtape!$B11)</f>
+        <v>75</v>
+      </c>
+      <c r="I12">
+        <f>SUM(B12:H12)</f>
+        <v>465</v>
+      </c>
+      <c r="J12">
+        <f>I12*$J$2</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>IF(B$2 = "FULL", Etape!$B12,DemiEtape!$B12)</f>
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <f>IF(C$2 = "FULL", Etape!$B12,DemiEtape!$B12)</f>
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <f>IF(D$2 = "FULL", Etape!$B12,DemiEtape!$B12)</f>
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <f>IF(E$2 = "FULL", Etape!$B12,DemiEtape!$B12)</f>
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <f>IF(F$2 = "FULL", Etape!$B12,DemiEtape!$B12)</f>
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <f>IF(G$2 = "FULL", Etape!$B12,DemiEtape!$B12)</f>
+        <v>30</v>
+      </c>
+      <c r="H13">
+        <f>IF(H$2 = "FULL", Etape!$B12,DemiEtape!$B12)</f>
+        <v>30</v>
+      </c>
+      <c r="I13">
+        <f>SUM(B13:H13)</f>
+        <v>210</v>
+      </c>
+      <c r="J13">
+        <f>I13*$J$2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>IF(B$2 = "FULL", Etape!$B13,DemiEtape!$B13)</f>
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <f>IF(C$2 = "FULL", Etape!$B13,DemiEtape!$B13)</f>
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <f>IF(D$2 = "FULL", Etape!$B13,DemiEtape!$B13)</f>
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <f>IF(E$2 = "FULL", Etape!$B13,DemiEtape!$B13)</f>
+        <v>30</v>
+      </c>
+      <c r="F14">
+        <f>IF(F$2 = "FULL", Etape!$B13,DemiEtape!$B13)</f>
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <f>IF(G$2 = "FULL", Etape!$B13,DemiEtape!$B13)</f>
+        <v>30</v>
+      </c>
+      <c r="H14">
+        <f>IF(H$2 = "FULL", Etape!$B13,DemiEtape!$B13)</f>
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <f>SUM(B14:H14)</f>
+        <v>210</v>
+      </c>
+      <c r="J14">
+        <f>I14*$J$2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f>IF(B$2 = "FULL", Etape!$B14,DemiEtape!$B14)</f>
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <f>IF(C$2 = "FULL", Etape!$B14,DemiEtape!$B14)</f>
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <f>IF(D$2 = "FULL", Etape!$B14,DemiEtape!$B14)</f>
+        <v>30</v>
+      </c>
+      <c r="E15">
+        <f>IF(E$2 = "FULL", Etape!$B14,DemiEtape!$B14)</f>
+        <v>30</v>
+      </c>
+      <c r="F15">
+        <f>IF(F$2 = "FULL", Etape!$B14,DemiEtape!$B14)</f>
+        <v>30</v>
+      </c>
+      <c r="G15">
+        <f>IF(G$2 = "FULL", Etape!$B14,DemiEtape!$B14)</f>
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <f>IF(H$2 = "FULL", Etape!$B14,DemiEtape!$B14)</f>
+        <v>30</v>
+      </c>
+      <c r="I15">
+        <f>SUM(B15:H15)</f>
+        <v>210</v>
+      </c>
+      <c r="J15">
+        <f>I15*$J$2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f>IF(B$2 = "FULL", Etape!$B15,DemiEtape!$B15)</f>
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <f>IF(C$2 = "FULL", Etape!$B15,DemiEtape!$B15)</f>
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <f>IF(D$2 = "FULL", Etape!$B15,DemiEtape!$B15)</f>
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <f>IF(E$2 = "FULL", Etape!$B15,DemiEtape!$B15)</f>
+        <v>30</v>
+      </c>
+      <c r="F16">
+        <f>IF(F$2 = "FULL", Etape!$B15,DemiEtape!$B15)</f>
+        <v>30</v>
+      </c>
+      <c r="G16">
+        <f>IF(G$2 = "FULL", Etape!$B15,DemiEtape!$B15)</f>
+        <v>30</v>
+      </c>
+      <c r="H16">
+        <f>IF(H$2 = "FULL", Etape!$B15,DemiEtape!$B15)</f>
+        <v>30</v>
+      </c>
+      <c r="I16">
+        <f>SUM(B16:H16)</f>
+        <v>210</v>
+      </c>
+      <c r="J16">
+        <f>I16*$J$2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f>IF(B$2 = "FULL", Etape!$B16,DemiEtape!$B16)</f>
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <f>IF(C$2 = "FULL", Etape!$B16,DemiEtape!$B16)</f>
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <f>IF(D$2 = "FULL", Etape!$B16,DemiEtape!$B16)</f>
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <f>IF(E$2 = "FULL", Etape!$B16,DemiEtape!$B16)</f>
+        <v>30</v>
+      </c>
+      <c r="F17">
+        <f>IF(F$2 = "FULL", Etape!$B16,DemiEtape!$B16)</f>
+        <v>30</v>
+      </c>
+      <c r="G17">
+        <f>IF(G$2 = "FULL", Etape!$B16,DemiEtape!$B16)</f>
+        <v>30</v>
+      </c>
+      <c r="H17">
+        <f>IF(H$2 = "FULL", Etape!$B16,DemiEtape!$B16)</f>
+        <v>30</v>
+      </c>
+      <c r="I17">
+        <f>SUM(B17:H17)</f>
+        <v>210</v>
+      </c>
+      <c r="J17">
+        <f>I17*$J$2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f>IF(B$2 = "FULL", Etape!$B17,DemiEtape!$B17)</f>
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <f>IF(C$2 = "FULL", Etape!$B17,DemiEtape!$B17)</f>
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <f>IF(D$2 = "FULL", Etape!$B17,DemiEtape!$B17)</f>
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <f>IF(E$2 = "FULL", Etape!$B17,DemiEtape!$B17)</f>
+        <v>30</v>
+      </c>
+      <c r="F18">
+        <f>IF(F$2 = "FULL", Etape!$B17,DemiEtape!$B17)</f>
+        <v>30</v>
+      </c>
+      <c r="G18">
+        <f>IF(G$2 = "FULL", Etape!$B17,DemiEtape!$B17)</f>
+        <v>30</v>
+      </c>
+      <c r="H18">
+        <f>IF(H$2 = "FULL", Etape!$B17,DemiEtape!$B17)</f>
+        <v>30</v>
+      </c>
+      <c r="I18">
+        <f>SUM(B18:H18)</f>
+        <v>210</v>
+      </c>
+      <c r="J18">
+        <f>I18*$J$2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f>IF(B$2 = "FULL", Etape!$B18,DemiEtape!$B18)</f>
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <f>IF(C$2 = "FULL", Etape!$B18,DemiEtape!$B18)</f>
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <f>IF(D$2 = "FULL", Etape!$B18,DemiEtape!$B18)</f>
+        <v>30</v>
+      </c>
+      <c r="E19">
+        <f>IF(E$2 = "FULL", Etape!$B18,DemiEtape!$B18)</f>
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <f>IF(F$2 = "FULL", Etape!$B18,DemiEtape!$B18)</f>
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <f>IF(G$2 = "FULL", Etape!$B18,DemiEtape!$B18)</f>
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <f>IF(H$2 = "FULL", Etape!$B18,DemiEtape!$B18)</f>
+        <v>30</v>
+      </c>
+      <c r="I19">
+        <f>SUM(B19:H19)</f>
+        <v>210</v>
+      </c>
+      <c r="J19">
+        <f>I19*$J$2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f>IF(B$2 = "FULL", Etape!$B19,DemiEtape!$B19)</f>
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <f>IF(C$2 = "FULL", Etape!$B19,DemiEtape!$B19)</f>
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <f>IF(D$2 = "FULL", Etape!$B19,DemiEtape!$B19)</f>
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <f>IF(E$2 = "FULL", Etape!$B19,DemiEtape!$B19)</f>
+        <v>30</v>
+      </c>
+      <c r="F20">
+        <f>IF(F$2 = "FULL", Etape!$B19,DemiEtape!$B19)</f>
+        <v>30</v>
+      </c>
+      <c r="G20">
+        <f>IF(G$2 = "FULL", Etape!$B19,DemiEtape!$B19)</f>
+        <v>30</v>
+      </c>
+      <c r="H20">
+        <f>IF(H$2 = "FULL", Etape!$B19,DemiEtape!$B19)</f>
+        <v>30</v>
+      </c>
+      <c r="I20">
+        <f>SUM(B20:H20)</f>
+        <v>210</v>
+      </c>
+      <c r="J20">
+        <f>I20*$J$2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f>IF(B$2 = "FULL", Etape!$B20,DemiEtape!$B20)</f>
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <f>IF(C$2 = "FULL", Etape!$B20,DemiEtape!$B20)</f>
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <f>IF(D$2 = "FULL", Etape!$B20,DemiEtape!$B20)</f>
+        <v>30</v>
+      </c>
+      <c r="E21">
+        <f>IF(E$2 = "FULL", Etape!$B20,DemiEtape!$B20)</f>
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <f>IF(F$2 = "FULL", Etape!$B20,DemiEtape!$B20)</f>
+        <v>30</v>
+      </c>
+      <c r="G21">
+        <f>IF(G$2 = "FULL", Etape!$B20,DemiEtape!$B20)</f>
+        <v>30</v>
+      </c>
+      <c r="H21">
+        <f>IF(H$2 = "FULL", Etape!$B20,DemiEtape!$B20)</f>
+        <v>30</v>
+      </c>
+      <c r="I21">
+        <f>SUM(B21:H21)</f>
+        <v>210</v>
+      </c>
+      <c r="J21">
+        <f>I21*$J$2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f>IF(B$2 = "FULL", Etape!$B21,DemiEtape!$B21)</f>
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <f>IF(C$2 = "FULL", Etape!$B21,DemiEtape!$B21)</f>
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <f>IF(D$2 = "FULL", Etape!$B21,DemiEtape!$B21)</f>
+        <v>30</v>
+      </c>
+      <c r="E22">
+        <f>IF(E$2 = "FULL", Etape!$B21,DemiEtape!$B21)</f>
+        <v>30</v>
+      </c>
+      <c r="F22">
+        <f>IF(F$2 = "FULL", Etape!$B21,DemiEtape!$B21)</f>
+        <v>30</v>
+      </c>
+      <c r="G22">
+        <f>IF(G$2 = "FULL", Etape!$B21,DemiEtape!$B21)</f>
+        <v>30</v>
+      </c>
+      <c r="H22">
+        <f>IF(H$2 = "FULL", Etape!$B21,DemiEtape!$B21)</f>
+        <v>30</v>
+      </c>
+      <c r="I22">
+        <f>SUM(B22:H22)</f>
+        <v>210</v>
+      </c>
+      <c r="J22">
+        <f>I22*$J$2</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <f>SUM(I3:I22)</f>
+        <v>8670</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.4487000000000001</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A32" r:id="rId1" xr:uid="{E5D767CF-292E-DC4B-BC13-706ECDC64A88}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87069C4E-32B1-BC46-A3D7-E19804EE9E33}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>145</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3">
+        <f>ROUNDUP(C2*Verif_UCI!$B$29,0)</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3" s="3">
+        <f>ROUNDUP(C3*Verif_UCI!$B$29,0)</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4" s="3">
+        <f>ROUNDUP(C4*Verif_UCI!$B$29,0)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5" s="3">
+        <f>ROUNDUP(C5*Verif_UCI!$B$29,0)</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3">
+        <f>ROUNDUP(C6*Verif_UCI!$B$29,0)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -726,17 +2022,33 @@
         <f>B6</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f>C6</f>
+        <v>30</v>
+      </c>
+      <c r="D7" s="3">
+        <f>ROUNDUP(C7*Verif_UCI!$B$29,0)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B11" si="0">B7</f>
+        <f t="shared" ref="B8:C11" si="0">B7</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <f>ROUNDUP(C8*Verif_UCI!$B$29,0)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -744,8 +2056,16 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D9" s="3">
+        <f>ROUNDUP(C9*Verif_UCI!$B$29,0)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -753,8 +2073,16 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D10" s="3">
+        <f>ROUNDUP(C10*Verif_UCI!$B$29,0)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -762,16 +2090,31 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D11" s="3">
+        <f>ROUNDUP(C11*Verif_UCI!$B$29,0)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3">
+        <f>ROUNDUP(C12*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -779,17 +2122,33 @@
         <f>B12</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f>C12</f>
+        <v>20</v>
+      </c>
+      <c r="D13" s="3">
+        <f>ROUNDUP(C13*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:B21" si="1">B13</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <f t="shared" ref="B14:C21" si="1">B13</f>
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D14" s="3">
+        <f>ROUNDUP(C14*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -797,8 +2156,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D15" s="3">
+        <f>ROUNDUP(C15*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -806,8 +2173,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D16" s="3">
+        <f>ROUNDUP(C16*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -815,8 +2190,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D17" s="3">
+        <f>ROUNDUP(C17*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -824,8 +2207,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D18" s="3">
+        <f>ROUNDUP(C18*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -833,8 +2224,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D19" s="3">
+        <f>ROUNDUP(C19*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -842,8 +2241,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D20" s="3">
+        <f>ROUNDUP(C20*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -851,8 +2258,16 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D21" s="3">
+        <f>ROUNDUP(C21*Verif_UCI!$B$29,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -862,6 +2277,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B21">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>B2-D2 &lt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -869,186 +2289,270 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1BBDAC-8CD5-9545-9088-974349703FED}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>400</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <f>Verif_UCI!J3</f>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <f>Verif_UCI!J4</f>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>150</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <f>Verif_UCI!J5</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <f>Verif_UCI!J6</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>95</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <f>Verif_UCI!J7</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f>Verif_UCI!J8</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>95</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <f>Verif_UCI!J9</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f>Verif_UCI!J10</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>95</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f>Verif_UCI!J11</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>95</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f>Verif_UCI!J12</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <f>Verif_UCI!J13</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f>Verif_UCI!J14</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f>Verif_UCI!J15</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f>Verif_UCI!J16</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f>Verif_UCI!J17</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f>Verif_UCI!J18</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f>Verif_UCI!J19</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f>Verif_UCI!J20</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f>Verif_UCI!J21</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f>Verif_UCI!J22</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1058,6 +2562,16 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C221">
+    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="greaterThan">
+      <formula>$B$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B21">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>B2-C2 &lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1349,15 +2863,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E71084-E10A-A54B-8C7F-0326267E2C80}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1371,7 +2885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1387,7 +2901,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1399,11 +2913,11 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D9" si="0">B3*C3</f>
+        <f>B3*C3</f>
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1415,11 +2929,11 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>B4*C4</f>
         <v>480</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1431,11 +2945,11 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>B5*C5</f>
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1447,11 +2961,11 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6" si="1">B6*C6</f>
+        <f>B6*C6</f>
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1463,11 +2977,11 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f>B7*C7</f>
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1479,11 +2993,12 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f>B8*C8</f>
         <v>6750</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1495,11 +3010,12 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f>B9*C9</f>
         <v>1920</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Corrections coquille fichier excel prix.
</commit_message>
<xml_diff>
--- a/excel/prix.xlsx
+++ b/excel/prix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCD025C-0CF2-3348-A65C-EB9EE195998C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8544C1B4-92C5-B24E-AA4E-4C4F46C0E9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="560" windowWidth="33480" windowHeight="20380" activeTab="9" xr2:uid="{CE5E1F58-89A2-BD42-AA5E-6DDAA3F3C6F4}"/>
   </bookViews>
@@ -976,7 +976,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,11 +1075,11 @@
         <v>255</v>
       </c>
       <c r="I3">
-        <f>SUM(B3:H3)</f>
+        <f t="shared" ref="I3:I22" si="0">SUM(B3:H3)</f>
         <v>1565</v>
       </c>
       <c r="J3">
-        <f>I3*$J$2</f>
+        <f t="shared" ref="J3:J22" si="1">I3*$J$2</f>
         <v>313</v>
       </c>
     </row>
@@ -1116,11 +1116,11 @@
         <v>145</v>
       </c>
       <c r="I4">
-        <f>SUM(B4:H4)</f>
+        <f t="shared" si="0"/>
         <v>945</v>
       </c>
       <c r="J4">
-        <f>I4*$J$2</f>
+        <f t="shared" si="1"/>
         <v>189</v>
       </c>
     </row>
@@ -1157,11 +1157,11 @@
         <v>110</v>
       </c>
       <c r="I5">
-        <f>SUM(B5:H5)</f>
+        <f t="shared" si="0"/>
         <v>700</v>
       </c>
       <c r="J5">
-        <f>I5*$J$2</f>
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
     </row>
@@ -1198,11 +1198,11 @@
         <v>90</v>
       </c>
       <c r="I6">
-        <f>SUM(B6:H6)</f>
+        <f t="shared" si="0"/>
         <v>570</v>
       </c>
       <c r="J6">
-        <f>I6*$J$2</f>
+        <f t="shared" si="1"/>
         <v>114</v>
       </c>
     </row>
@@ -1239,11 +1239,11 @@
         <v>75</v>
       </c>
       <c r="I7">
-        <f>SUM(B7:H7)</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
       <c r="J7">
-        <f>I7*$J$2</f>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
@@ -1280,11 +1280,11 @@
         <v>75</v>
       </c>
       <c r="I8">
-        <f>SUM(B8:H8)</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
       <c r="J8">
-        <f>I8*$J$2</f>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
@@ -1321,11 +1321,11 @@
         <v>75</v>
       </c>
       <c r="I9">
-        <f>SUM(B9:H9)</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
       <c r="J9">
-        <f>I9*$J$2</f>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
@@ -1362,11 +1362,11 @@
         <v>75</v>
       </c>
       <c r="I10">
-        <f>SUM(B10:H10)</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
       <c r="J10">
-        <f>I10*$J$2</f>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
@@ -1403,11 +1403,11 @@
         <v>75</v>
       </c>
       <c r="I11">
-        <f>SUM(B11:H11)</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
       <c r="J11">
-        <f>I11*$J$2</f>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
@@ -1444,11 +1444,11 @@
         <v>75</v>
       </c>
       <c r="I12">
-        <f>SUM(B12:H12)</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
       <c r="J12">
-        <f>I12*$J$2</f>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
@@ -1485,11 +1485,11 @@
         <v>30</v>
       </c>
       <c r="I13">
-        <f>SUM(B13:H13)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="J13">
-        <f>I13*$J$2</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -1526,11 +1526,11 @@
         <v>30</v>
       </c>
       <c r="I14">
-        <f>SUM(B14:H14)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="J14">
-        <f>I14*$J$2</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -1567,11 +1567,11 @@
         <v>30</v>
       </c>
       <c r="I15">
-        <f>SUM(B15:H15)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="J15">
-        <f>I15*$J$2</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -1608,11 +1608,11 @@
         <v>30</v>
       </c>
       <c r="I16">
-        <f>SUM(B16:H16)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="J16">
-        <f>I16*$J$2</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -1649,11 +1649,11 @@
         <v>30</v>
       </c>
       <c r="I17">
-        <f>SUM(B17:H17)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="J17">
-        <f>I17*$J$2</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -1690,11 +1690,11 @@
         <v>30</v>
       </c>
       <c r="I18">
-        <f>SUM(B18:H18)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="J18">
-        <f>I18*$J$2</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -1731,11 +1731,11 @@
         <v>30</v>
       </c>
       <c r="I19">
-        <f>SUM(B19:H19)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="J19">
-        <f>I19*$J$2</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -1772,11 +1772,11 @@
         <v>30</v>
       </c>
       <c r="I20">
-        <f>SUM(B20:H20)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="J20">
-        <f>I20*$J$2</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -1813,11 +1813,11 @@
         <v>30</v>
       </c>
       <c r="I21">
-        <f>SUM(B21:H21)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="J21">
-        <f>I21*$J$2</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -1854,11 +1854,11 @@
         <v>30</v>
       </c>
       <c r="I22">
-        <f>SUM(B22:H22)</f>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="J22">
-        <f>I22*$J$2</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -1907,6 +1907,7 @@
     <hyperlink ref="A32" r:id="rId1" xr:uid="{E5D767CF-292E-DC4B-BC13-706ECDC64A88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2897,7 +2898,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f>B2*C2</f>
+        <f t="shared" ref="D2:D9" si="0">B2*C2</f>
         <v>1885</v>
       </c>
     </row>
@@ -2913,7 +2914,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f>B3*C3</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
@@ -2929,7 +2930,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <f>B4*C4</f>
+        <f t="shared" si="0"/>
         <v>480</v>
       </c>
     </row>
@@ -2945,7 +2946,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <f>B5*C5</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
@@ -2961,7 +2962,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <f>B6*C6</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
@@ -2977,7 +2978,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <f>B7*C7</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
@@ -2993,7 +2994,7 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <f>B8*C8</f>
+        <f t="shared" si="0"/>
         <v>6750</v>
       </c>
       <c r="E8" s="5"/>
@@ -3010,7 +3011,7 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <f>B9*C9</f>
+        <f t="shared" si="0"/>
         <v>1920</v>
       </c>
       <c r="E9" s="5"/>

</xml_diff>